<commit_message>
I added the properties in each class of Opendss, when empty
</commit_message>
<xml_diff>
--- a/py_fx_tools_dss/IMEX_to_DSS/xlsx_DSS_xlsx/Examples/13NodeIEEE/BBDD_DSS_default.xlsx
+++ b/py_fx_tools_dss/IMEX_to_DSS/xlsx_DSS_xlsx/Examples/13NodeIEEE/BBDD_DSS_default.xlsx
@@ -33,27 +33,31 @@
     <sheet name="CapControl" sheetId="24" state="visible" r:id="rId24"/>
     <sheet name="Fault" sheetId="25" state="visible" r:id="rId25"/>
     <sheet name="Generator" sheetId="26" state="visible" r:id="rId26"/>
-    <sheet name="GenDispatcher" sheetId="27" state="visible" r:id="rId27"/>
-    <sheet name="Storage" sheetId="28" state="visible" r:id="rId28"/>
-    <sheet name="StorageController" sheetId="29" state="visible" r:id="rId29"/>
-    <sheet name="Relay" sheetId="30" state="visible" r:id="rId30"/>
-    <sheet name="Recloser" sheetId="31" state="visible" r:id="rId31"/>
-    <sheet name="Fuse" sheetId="32" state="visible" r:id="rId32"/>
-    <sheet name="SwtControl" sheetId="33" state="visible" r:id="rId33"/>
-    <sheet name="PVSystem" sheetId="34" state="visible" r:id="rId34"/>
-    <sheet name="UPFC" sheetId="35" state="visible" r:id="rId35"/>
-    <sheet name="UPFCControl" sheetId="36" state="visible" r:id="rId36"/>
-    <sheet name="ESPVLControl" sheetId="37" state="visible" r:id="rId37"/>
-    <sheet name="IndMach012" sheetId="38" state="visible" r:id="rId38"/>
-    <sheet name="GICsource" sheetId="39" state="visible" r:id="rId39"/>
-    <sheet name="AutoTrans" sheetId="40" state="visible" r:id="rId40"/>
-    <sheet name="InvControl" sheetId="41" state="visible" r:id="rId41"/>
-    <sheet name="ExpControl" sheetId="42" state="visible" r:id="rId42"/>
-    <sheet name="GICTransformer" sheetId="43" state="visible" r:id="rId43"/>
-    <sheet name="VSConverter" sheetId="44" state="visible" r:id="rId44"/>
-    <sheet name="Monitor" sheetId="45" state="visible" r:id="rId45"/>
-    <sheet name="EnergyMeter" sheetId="46" state="visible" r:id="rId46"/>
-    <sheet name="Sensor" sheetId="47" state="visible" r:id="rId47"/>
+    <sheet name="WindGen" sheetId="27" state="visible" r:id="rId27"/>
+    <sheet name="GenDispatcher" sheetId="28" state="visible" r:id="rId28"/>
+    <sheet name="Storage" sheetId="29" state="visible" r:id="rId29"/>
+    <sheet name="StorageController" sheetId="30" state="visible" r:id="rId30"/>
+    <sheet name="Relay" sheetId="31" state="visible" r:id="rId31"/>
+    <sheet name="Recloser" sheetId="32" state="visible" r:id="rId32"/>
+    <sheet name="Fuse" sheetId="33" state="visible" r:id="rId33"/>
+    <sheet name="SwtControl" sheetId="34" state="visible" r:id="rId34"/>
+    <sheet name="PVSystem" sheetId="35" state="visible" r:id="rId35"/>
+    <sheet name="UPFC" sheetId="36" state="visible" r:id="rId36"/>
+    <sheet name="UPFCControl" sheetId="37" state="visible" r:id="rId37"/>
+    <sheet name="ESPVLControl" sheetId="38" state="visible" r:id="rId38"/>
+    <sheet name="IndMach012" sheetId="39" state="visible" r:id="rId39"/>
+    <sheet name="GICsource" sheetId="40" state="visible" r:id="rId40"/>
+    <sheet name="AutoTrans" sheetId="41" state="visible" r:id="rId41"/>
+    <sheet name="InvControl" sheetId="42" state="visible" r:id="rId42"/>
+    <sheet name="ExpControl" sheetId="43" state="visible" r:id="rId43"/>
+    <sheet name="GICLine" sheetId="44" state="visible" r:id="rId44"/>
+    <sheet name="GICTransformer" sheetId="45" state="visible" r:id="rId45"/>
+    <sheet name="VSConverter" sheetId="46" state="visible" r:id="rId46"/>
+    <sheet name="Monitor" sheetId="47" state="visible" r:id="rId47"/>
+    <sheet name="EnergyMeter" sheetId="48" state="visible" r:id="rId48"/>
+    <sheet name="Sensor" sheetId="49" state="visible" r:id="rId49"/>
+    <sheet name="FMonitor" sheetId="50" state="visible" r:id="rId50"/>
+    <sheet name="Generic5" sheetId="51" state="visible" r:id="rId51"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -16008,7 +16012,7 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>('0 |1.87639338887875E-310 2.25607960651843E-308 |6.25928299106659E-306 0 6.25926796099676E-306',)</t>
+          <t>('0 |1.87639338887875E-310 2.25607960651843E-308 |1.15409172934718E-305 0 1.15409061474694E-305',)</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
@@ -17072,7 +17076,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Id_GenDispatcher</t>
+          <t>Id_WindGen</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -17288,7 +17292,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Id_Storage</t>
+          <t>Id_GenDispatcher</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -17504,7 +17508,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Id_StorageController</t>
+          <t>Id_Storage</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -17936,7 +17940,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Id_Relay</t>
+          <t>Id_StorageController</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -18152,7 +18156,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Id_Recloser</t>
+          <t>Id_Relay</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -18368,7 +18372,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Id_Fuse</t>
+          <t>Id_Recloser</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -18584,7 +18588,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Id_SwtControl</t>
+          <t>Id_Fuse</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -18800,7 +18804,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Id_PVSystem</t>
+          <t>Id_SwtControl</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -19016,7 +19020,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Id_UPFC</t>
+          <t>Id_PVSystem</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -19232,7 +19236,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Id_UPFCControl</t>
+          <t>Id_UPFC</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -19448,7 +19452,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Id_ESPVLControl</t>
+          <t>Id_UPFCControl</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -19664,7 +19668,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Id_IndMach012</t>
+          <t>Id_ESPVLControl</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -19880,7 +19884,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Id_GICsource</t>
+          <t>Id_IndMach012</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -20312,7 +20316,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Id_AutoTrans</t>
+          <t>Id_GICsource</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -20528,7 +20532,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Id_InvControl</t>
+          <t>Id_AutoTrans</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -20744,7 +20748,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Id_ExpControl</t>
+          <t>Id_InvControl</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -20960,7 +20964,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Id_GICTransformer</t>
+          <t>Id_ExpControl</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -21176,7 +21180,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Id_VSConverter</t>
+          <t>Id_GICLine</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -21392,7 +21396,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Id_Monitor</t>
+          <t>Id_GICTransformer</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -21608,7 +21612,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Id_EnergyMeter</t>
+          <t>Id_VSConverter</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -21824,6 +21828,438 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>Id_Monitor</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>bus1</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>bus2</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>linecode</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>length</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>phases</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>r1</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>x1</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>r0</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>x0</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>C0</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>rmatrix</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>xmatrix</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>cmatrix</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Switch</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>Rg</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>Xg</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>rho</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>geometry</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>units</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>spacing</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>wires</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>EarthModel</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>cncables</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>tscables</t>
+        </is>
+      </c>
+      <c r="AA1" s="1" t="inlineStr">
+        <is>
+          <t>B1</t>
+        </is>
+      </c>
+      <c r="AB1" s="1" t="inlineStr">
+        <is>
+          <t>B0</t>
+        </is>
+      </c>
+      <c r="AC1" s="1" t="inlineStr">
+        <is>
+          <t>Seasons</t>
+        </is>
+      </c>
+      <c r="AD1" s="1" t="inlineStr">
+        <is>
+          <t>Ratings</t>
+        </is>
+      </c>
+      <c r="AE1" s="1" t="inlineStr">
+        <is>
+          <t>LineType</t>
+        </is>
+      </c>
+      <c r="AF1" s="1" t="inlineStr">
+        <is>
+          <t>normamps</t>
+        </is>
+      </c>
+      <c r="AG1" s="1" t="inlineStr">
+        <is>
+          <t>emergamps</t>
+        </is>
+      </c>
+      <c r="AH1" s="1" t="inlineStr">
+        <is>
+          <t>faultrate</t>
+        </is>
+      </c>
+      <c r="AI1" s="1" t="inlineStr">
+        <is>
+          <t>pctperm</t>
+        </is>
+      </c>
+      <c r="AJ1" s="1" t="inlineStr">
+        <is>
+          <t>repair</t>
+        </is>
+      </c>
+      <c r="AK1" s="1" t="inlineStr">
+        <is>
+          <t>basefreq</t>
+        </is>
+      </c>
+      <c r="AL1" s="1" t="inlineStr">
+        <is>
+          <t>enabled</t>
+        </is>
+      </c>
+      <c r="AM1" s="1" t="inlineStr">
+        <is>
+          <t>like</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:AM1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Id_EnergyMeter</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>bus1</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>bus2</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>linecode</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>length</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>phases</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>r1</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>x1</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>r0</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>x0</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>C0</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>rmatrix</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>xmatrix</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>cmatrix</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Switch</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>Rg</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>Xg</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>rho</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>geometry</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>units</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>spacing</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>wires</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>EarthModel</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>cncables</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>tscables</t>
+        </is>
+      </c>
+      <c r="AA1" s="1" t="inlineStr">
+        <is>
+          <t>B1</t>
+        </is>
+      </c>
+      <c r="AB1" s="1" t="inlineStr">
+        <is>
+          <t>B0</t>
+        </is>
+      </c>
+      <c r="AC1" s="1" t="inlineStr">
+        <is>
+          <t>Seasons</t>
+        </is>
+      </c>
+      <c r="AD1" s="1" t="inlineStr">
+        <is>
+          <t>Ratings</t>
+        </is>
+      </c>
+      <c r="AE1" s="1" t="inlineStr">
+        <is>
+          <t>LineType</t>
+        </is>
+      </c>
+      <c r="AF1" s="1" t="inlineStr">
+        <is>
+          <t>normamps</t>
+        </is>
+      </c>
+      <c r="AG1" s="1" t="inlineStr">
+        <is>
+          <t>emergamps</t>
+        </is>
+      </c>
+      <c r="AH1" s="1" t="inlineStr">
+        <is>
+          <t>faultrate</t>
+        </is>
+      </c>
+      <c r="AI1" s="1" t="inlineStr">
+        <is>
+          <t>pctperm</t>
+        </is>
+      </c>
+      <c r="AJ1" s="1" t="inlineStr">
+        <is>
+          <t>repair</t>
+        </is>
+      </c>
+      <c r="AK1" s="1" t="inlineStr">
+        <is>
+          <t>basefreq</t>
+        </is>
+      </c>
+      <c r="AL1" s="1" t="inlineStr">
+        <is>
+          <t>enabled</t>
+        </is>
+      </c>
+      <c r="AM1" s="1" t="inlineStr">
+        <is>
+          <t>like</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:AM1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
           <t>Id_Sensor</t>
         </is>
       </c>
@@ -22041,6 +22477,438 @@
       <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Id_XYcurve</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>bus1</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>bus2</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>linecode</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>length</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>phases</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>r1</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>x1</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>r0</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>x0</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>C0</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>rmatrix</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>xmatrix</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>cmatrix</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Switch</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>Rg</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>Xg</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>rho</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>geometry</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>units</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>spacing</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>wires</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>EarthModel</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>cncables</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>tscables</t>
+        </is>
+      </c>
+      <c r="AA1" s="1" t="inlineStr">
+        <is>
+          <t>B1</t>
+        </is>
+      </c>
+      <c r="AB1" s="1" t="inlineStr">
+        <is>
+          <t>B0</t>
+        </is>
+      </c>
+      <c r="AC1" s="1" t="inlineStr">
+        <is>
+          <t>Seasons</t>
+        </is>
+      </c>
+      <c r="AD1" s="1" t="inlineStr">
+        <is>
+          <t>Ratings</t>
+        </is>
+      </c>
+      <c r="AE1" s="1" t="inlineStr">
+        <is>
+          <t>LineType</t>
+        </is>
+      </c>
+      <c r="AF1" s="1" t="inlineStr">
+        <is>
+          <t>normamps</t>
+        </is>
+      </c>
+      <c r="AG1" s="1" t="inlineStr">
+        <is>
+          <t>emergamps</t>
+        </is>
+      </c>
+      <c r="AH1" s="1" t="inlineStr">
+        <is>
+          <t>faultrate</t>
+        </is>
+      </c>
+      <c r="AI1" s="1" t="inlineStr">
+        <is>
+          <t>pctperm</t>
+        </is>
+      </c>
+      <c r="AJ1" s="1" t="inlineStr">
+        <is>
+          <t>repair</t>
+        </is>
+      </c>
+      <c r="AK1" s="1" t="inlineStr">
+        <is>
+          <t>basefreq</t>
+        </is>
+      </c>
+      <c r="AL1" s="1" t="inlineStr">
+        <is>
+          <t>enabled</t>
+        </is>
+      </c>
+      <c r="AM1" s="1" t="inlineStr">
+        <is>
+          <t>like</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet50.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:AM1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Id_FMonitor</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>bus1</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>bus2</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>linecode</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>length</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>phases</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>r1</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>x1</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>r0</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>x0</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>C0</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>rmatrix</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>xmatrix</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>cmatrix</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Switch</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>Rg</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>Xg</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>rho</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>geometry</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>units</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>spacing</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>wires</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>EarthModel</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>cncables</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>tscables</t>
+        </is>
+      </c>
+      <c r="AA1" s="1" t="inlineStr">
+        <is>
+          <t>B1</t>
+        </is>
+      </c>
+      <c r="AB1" s="1" t="inlineStr">
+        <is>
+          <t>B0</t>
+        </is>
+      </c>
+      <c r="AC1" s="1" t="inlineStr">
+        <is>
+          <t>Seasons</t>
+        </is>
+      </c>
+      <c r="AD1" s="1" t="inlineStr">
+        <is>
+          <t>Ratings</t>
+        </is>
+      </c>
+      <c r="AE1" s="1" t="inlineStr">
+        <is>
+          <t>LineType</t>
+        </is>
+      </c>
+      <c r="AF1" s="1" t="inlineStr">
+        <is>
+          <t>normamps</t>
+        </is>
+      </c>
+      <c r="AG1" s="1" t="inlineStr">
+        <is>
+          <t>emergamps</t>
+        </is>
+      </c>
+      <c r="AH1" s="1" t="inlineStr">
+        <is>
+          <t>faultrate</t>
+        </is>
+      </c>
+      <c r="AI1" s="1" t="inlineStr">
+        <is>
+          <t>pctperm</t>
+        </is>
+      </c>
+      <c r="AJ1" s="1" t="inlineStr">
+        <is>
+          <t>repair</t>
+        </is>
+      </c>
+      <c r="AK1" s="1" t="inlineStr">
+        <is>
+          <t>basefreq</t>
+        </is>
+      </c>
+      <c r="AL1" s="1" t="inlineStr">
+        <is>
+          <t>enabled</t>
+        </is>
+      </c>
+      <c r="AM1" s="1" t="inlineStr">
+        <is>
+          <t>like</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:AM1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Id_Generic5</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">

</xml_diff>